<commit_message>
3d plots working in runAll
</commit_message>
<xml_diff>
--- a/PracticeData.xlsx
+++ b/PracticeData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="26">
   <si>
     <t>Time</t>
   </si>
@@ -70,6 +70,30 @@
   </si>
   <si>
     <t>StdDeviation</t>
+  </si>
+  <si>
+    <t>Cat3</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>Z</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>V</t>
   </si>
 </sst>
 </file>
@@ -408,15 +432,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I32"/>
+  <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -444,8 +468,11 @@
       <c r="I1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <f>1</f>
         <v>1</v>
@@ -474,8 +501,11 @@
       <c r="I2">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <f>A2+1</f>
         <v>2</v>
@@ -507,8 +537,11 @@
       <c r="I3">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <f t="shared" ref="A4:A32" si="3">A3+1</f>
         <v>3</v>
@@ -540,8 +573,11 @@
       <c r="I4">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" si="3"/>
         <v>4</v>
@@ -573,8 +609,11 @@
       <c r="I5">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" si="3"/>
         <v>5</v>
@@ -605,8 +644,11 @@
       <c r="I6">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" si="3"/>
         <v>6</v>
@@ -638,8 +680,11 @@
       <c r="I7">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" si="3"/>
         <v>7</v>
@@ -671,8 +716,11 @@
       <c r="I8">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" si="3"/>
         <v>8</v>
@@ -704,8 +752,11 @@
       <c r="I9">
         <v>5</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" si="3"/>
         <v>9</v>
@@ -737,8 +788,11 @@
       <c r="I10">
         <v>5</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" si="3"/>
         <v>10</v>
@@ -770,8 +824,11 @@
       <c r="I11">
         <v>5</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" si="3"/>
         <v>11</v>
@@ -803,8 +860,11 @@
       <c r="I12">
         <v>5</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13">
         <f t="shared" si="3"/>
         <v>12</v>
@@ -836,8 +896,11 @@
       <c r="I13">
         <v>5</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14">
         <f t="shared" si="3"/>
         <v>13</v>
@@ -869,8 +932,11 @@
       <c r="I14">
         <v>5</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J14" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15">
         <f t="shared" si="3"/>
         <v>14</v>
@@ -902,8 +968,11 @@
       <c r="I15">
         <v>5</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16">
         <f t="shared" si="3"/>
         <v>15</v>
@@ -935,8 +1004,11 @@
       <c r="I16">
         <v>64</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17">
         <f t="shared" si="3"/>
         <v>16</v>
@@ -965,8 +1037,11 @@
       <c r="I17">
         <v>5</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J17" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18">
         <f t="shared" si="3"/>
         <v>17</v>
@@ -997,8 +1072,11 @@
       <c r="I18">
         <v>5</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J18" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19">
         <f t="shared" si="3"/>
         <v>18</v>
@@ -1028,8 +1106,11 @@
       <c r="I19">
         <v>5</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J19" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20">
         <f>A19+1</f>
         <v>19</v>
@@ -1060,8 +1141,11 @@
       <c r="I20">
         <v>5</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J20" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21">
         <f t="shared" si="3"/>
         <v>20</v>
@@ -1092,8 +1176,11 @@
       <c r="I21">
         <v>5</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J21" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22">
         <f t="shared" si="3"/>
         <v>21</v>
@@ -1120,8 +1207,11 @@
       <c r="I22">
         <v>5</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J22" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23">
         <f t="shared" si="3"/>
         <v>22</v>
@@ -1152,8 +1242,11 @@
       <c r="I23">
         <v>5</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J23" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24">
         <f t="shared" si="3"/>
         <v>23</v>
@@ -1184,8 +1277,11 @@
       <c r="I24">
         <v>5</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J24" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25">
         <f t="shared" si="3"/>
         <v>24</v>
@@ -1213,8 +1309,11 @@
       <c r="I25">
         <v>5</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J25" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26">
         <f t="shared" si="3"/>
         <v>25</v>
@@ -1245,8 +1344,11 @@
       <c r="I26">
         <v>5</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J26" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27">
         <f t="shared" si="3"/>
         <v>26</v>
@@ -1277,8 +1379,11 @@
       <c r="I27">
         <v>5</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J27" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28">
         <f t="shared" si="3"/>
         <v>27</v>
@@ -1309,8 +1414,11 @@
       <c r="I28">
         <v>5</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J28" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29">
         <f t="shared" si="3"/>
         <v>28</v>
@@ -1338,8 +1446,11 @@
       <c r="I29">
         <v>5</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J29" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30">
         <f t="shared" si="3"/>
         <v>29</v>
@@ -1370,8 +1481,11 @@
       <c r="I30">
         <v>5</v>
       </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J30" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31">
         <f t="shared" si="3"/>
         <v>30</v>
@@ -1402,8 +1516,11 @@
       <c r="I31">
         <v>5</v>
       </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J31" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32">
         <f t="shared" si="3"/>
         <v>31</v>
@@ -1433,6 +1550,9 @@
       </c>
       <c r="I32">
         <v>5</v>
+      </c>
+      <c r="J32" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>